<commit_message>
new bad images data updated
</commit_message>
<xml_diff>
--- a/Data/Processed/handcount_new_bad_images.xlsx
+++ b/Data/Processed/handcount_new_bad_images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngomae/MyGithub/h2lifespan/Data/Processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3A7E6D42-F452-2A48-8AA0-3D82C52C9301}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2DFF8A7C-2716-0843-A8AB-A7FBF3A1D806}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="3260" windowWidth="27140" windowHeight="16540" xr2:uid="{9ABC6890-52DA-674E-915C-0FD67EBFD82B}"/>
+    <workbookView xWindow="19180" yWindow="840" windowWidth="10580" windowHeight="16540" xr2:uid="{9ABC6890-52DA-674E-915C-0FD67EBFD82B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>camera_id</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>cms=count makes sense</t>
+  </si>
+  <si>
+    <t>pred. 131</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7C4DED-4450-A54E-8076-457DD1CCD8F0}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -409,23 +412,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>3719</v>
+        <v>2928</v>
       </c>
       <c r="B2">
+        <v>617</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3794</v>
+        <v>3160</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>612</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4953</v>
+        <v>3523</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -433,31 +439,31 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3721</v>
+        <v>3534</v>
       </c>
       <c r="B5">
-        <v>153</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5688</v>
+        <v>3568</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5641</v>
-      </c>
-      <c r="B7">
+        <v>3654</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>5672</v>
+        <v>3710</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -465,7 +471,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>4970</v>
+        <v>3719</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -473,47 +479,47 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>5180</v>
+        <v>3721</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>5674</v>
+        <v>3725</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>5187</v>
+        <v>3745</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>4310</v>
+        <v>3747</v>
       </c>
       <c r="B13">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>3747</v>
+        <v>3792</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>5676</v>
+        <v>3794</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -521,7 +527,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>3654</v>
+        <v>3815</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -529,39 +535,39 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>5438</v>
+        <v>4310</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>5662</v>
+        <v>4311</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>5647</v>
+        <v>4340</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>5555</v>
+        <v>4355</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>5525</v>
+        <v>4441</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -569,7 +575,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>5552</v>
+        <v>4511</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -577,15 +583,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5225</v>
+        <v>4929</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5564</v>
+        <v>4953</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -593,15 +599,15 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>5656</v>
+        <v>4970</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>3568</v>
+        <v>5057</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -609,7 +615,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>5637</v>
+        <v>5070</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -617,7 +623,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>5543</v>
+        <v>5148</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -625,29 +631,1092 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>4355</v>
+        <v>5180</v>
       </c>
       <c r="B29">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>3815</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
+        <v>5183</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>4511</v>
+        <v>5187</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>5189</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>5225</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5438</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>5454</v>
+      </c>
+      <c r="B35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>5486</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>5525</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>5543</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>5552</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>5555</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>5564</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>5607</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5637</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>5641</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>5642</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>5647</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>5656</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>5662</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>5672</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>5674</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>5676</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>5688</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5708</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>5710</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>5711</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>5720</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>5724</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>5728</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>5597</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>5598</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>5604</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>5605</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>5607</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>5608</v>
+      </c>
+      <c r="B65">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>5610</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>5611</v>
+      </c>
+      <c r="B67">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>5612</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>5613</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>5614</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>5615</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>5616</v>
+      </c>
+      <c r="B72">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>5619</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>5620</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>5621</v>
+      </c>
+      <c r="B75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>5622</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>5623</v>
+      </c>
+      <c r="B77">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>5624</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>5625</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>5626</v>
+      </c>
+      <c r="B80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>5627</v>
+      </c>
+      <c r="B81">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>5628</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>5629</v>
+      </c>
+      <c r="B83">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>5630</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>5631</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>5632</v>
+      </c>
+      <c r="B86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>5633</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>5634</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>5635</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>5636</v>
+      </c>
+      <c r="B90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>5637</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>5638</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>5639</v>
+      </c>
+      <c r="B93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>5640</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>5641</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>5642</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>5643</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>5644</v>
+      </c>
+      <c r="B98">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>5645</v>
+      </c>
+      <c r="B99">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>5646</v>
+      </c>
+      <c r="B100">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>5647</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>5648</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>5649</v>
+      </c>
+      <c r="B103">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>5650</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>5651</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>5652</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>5653</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>5654</v>
+      </c>
+      <c r="B108">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>5655</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>5656</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>5657</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>5658</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>5659</v>
+      </c>
+      <c r="B113">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>5660</v>
+      </c>
+      <c r="B114">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>5661</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>5662</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>5663</v>
+      </c>
+      <c r="B117">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>5664</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>5665</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>5666</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>5667</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>5668</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>5669</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>5670</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>5671</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>5672</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>5673</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>5674</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>5675</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>5676</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>5677</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>5678</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>5679</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>5680</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>5681</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>5682</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>5683</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>5684</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>5685</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>5686</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>5687</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>5688</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>5689</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>5690</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>5691</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>5692</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>5693</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>5694</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>5695</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>5696</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>5697</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>5698</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>5699</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>5701</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>5702</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>5703</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>5704</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>5705</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>5706</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>5707</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>5708</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>5709</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>5710</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>5711</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>5712</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>5713</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>5714</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>5715</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>5716</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>5717</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>5718</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>5719</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>5720</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>5721</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>5722</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>5723</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>5724</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>5725</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>5726</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>5727</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>5728</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>5729</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>5730</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>5731</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>5732</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>5733</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>5734</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>5735</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>5736</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>5737</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>5738</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>5739</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:C58">
+    <sortCondition ref="A2:A58"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new hand counts updated
</commit_message>
<xml_diff>
--- a/Data/Processed/handcount_new_bad_images.xlsx
+++ b/Data/Processed/handcount_new_bad_images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngomae/MyGithub/h2lifespan/Data/Processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2DFF8A7C-2716-0843-A8AB-A7FBF3A1D806}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{35C1C103-27FF-C641-8447-151FC2EF61CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19180" yWindow="840" windowWidth="10580" windowHeight="16540" xr2:uid="{9ABC6890-52DA-674E-915C-0FD67EBFD82B}"/>
+    <workbookView xWindow="16900" yWindow="1740" windowWidth="10580" windowHeight="16540" xr2:uid="{9ABC6890-52DA-674E-915C-0FD67EBFD82B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>camera_id</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>pred. 131</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7C4DED-4450-A54E-8076-457DD1CCD8F0}">
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,380 +1340,603 @@
       <c r="A118">
         <v>5664</v>
       </c>
+      <c r="B118">
+        <v>2</v>
+      </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>5665</v>
       </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>5666</v>
       </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>5667</v>
       </c>
+      <c r="B121">
+        <v>7</v>
+      </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>5668</v>
       </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>5669</v>
       </c>
+      <c r="B123">
+        <v>47</v>
+      </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>5670</v>
       </c>
+      <c r="B124">
+        <v>2</v>
+      </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>5671</v>
       </c>
+      <c r="B125">
+        <v>23</v>
+      </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>5672</v>
       </c>
+      <c r="B126">
+        <v>2</v>
+      </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>5673</v>
       </c>
+      <c r="B127">
+        <v>17</v>
+      </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>5674</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>5675</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>5676</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>5677</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>5678</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>5679</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>5680</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>5681</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>5682</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>5683</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>5684</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B138">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>5685</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>5686</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B140">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>5687</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>5688</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>5689</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B143">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>5690</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>5691</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B145">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>5692</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>5693</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>5694</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B148">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>5695</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>5696</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B150">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>5697</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B151">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>5698</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>5699</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B153">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>5700</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B154">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>5701</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B155">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>5702</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>5703</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>5704</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B158">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>5705</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>5706</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>5707</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>5708</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>5709</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>5710</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B164">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>5711</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>5712</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>5713</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B167">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>5714</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>5715</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B169">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>5716</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B170">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>5717</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B171">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>5718</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>5719</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>5720</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>5721</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>5722</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B176">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>5723</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B177">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>5724</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>5725</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>5726</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>5727</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>5728</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>5729</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>5730</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>5731</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>5732</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>5733</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>5734</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>5735</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>5736</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191">
-        <v>5737</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+        <v>5738</v>
+      </c>
+      <c r="B191" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192">
-        <v>5738</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A193">
         <v>5739</v>
+      </c>
+      <c r="B192" t="s">
+        <v>2</v>
+      </c>
+      <c r="C192">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a better version of new bad counts
</commit_message>
<xml_diff>
--- a/Data/Processed/handcount_new_bad_images.xlsx
+++ b/Data/Processed/handcount_new_bad_images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngomae/MyGithub/h2lifespan/Data/Processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{35C1C103-27FF-C641-8447-151FC2EF61CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC296401-8367-3444-AC5A-4B99494D581D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16900" yWindow="1740" windowWidth="10580" windowHeight="16540" xr2:uid="{9ABC6890-52DA-674E-915C-0FD67EBFD82B}"/>
+    <workbookView xWindow="5240" yWindow="1740" windowWidth="21960" windowHeight="16540" xr2:uid="{9ABC6890-52DA-674E-915C-0FD67EBFD82B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>camera_id</t>
   </si>
   <si>
     <t>count</t>
-  </si>
-  <si>
-    <t>cms</t>
-  </si>
-  <si>
-    <t>cms=count makes sense</t>
-  </si>
-  <si>
-    <t>pred. 131</t>
   </si>
   <si>
     <t>NA</t>
@@ -49,10 +40,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,8 +76,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,327 +393,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7C4DED-4450-A54E-8076-457DD1CCD8F0}">
-  <dimension ref="A1:C192"/>
+  <dimension ref="A1:B171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+      <selection activeCell="A172" sqref="A172:XFD172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>2928</v>
       </c>
       <c r="B2">
         <v>617</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>3160</v>
       </c>
       <c r="B3">
         <v>612</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>3523</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>3534</v>
       </c>
       <c r="B5">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>3568</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3654</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>3710</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>3719</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3721</v>
+      </c>
+      <c r="B9">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>3725</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>3745</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>3747</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>3792</v>
+      </c>
+      <c r="B13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>3794</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>4310</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>4311</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>4340</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>4355</v>
+      </c>
+      <c r="B18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>4441</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>4511</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>4929</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>4953</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>4970</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>5057</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>5070</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>5148</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>5180</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>5183</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>5187</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>5189</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>5225</v>
+      </c>
+      <c r="B31">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>3710</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>3719</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>3721</v>
-      </c>
-      <c r="B10">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>3725</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>3745</v>
-      </c>
-      <c r="B12">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>3747</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>3792</v>
-      </c>
-      <c r="B14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>3794</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>3815</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>5438</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>5454</v>
+      </c>
+      <c r="B33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>5486</v>
+      </c>
+      <c r="B34">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>4310</v>
-      </c>
-      <c r="B17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>4311</v>
-      </c>
-      <c r="B18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>4340</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>4355</v>
-      </c>
-      <c r="B20">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>4441</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>4511</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>4929</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>4953</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>4970</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>5057</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>5070</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>5148</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>5180</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>5183</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>5187</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>5189</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>5225</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>5438</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-    </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>5454</v>
+      <c r="A35" s="1">
+        <v>5525</v>
       </c>
       <c r="B35">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>5486</v>
+      <c r="A36" s="1">
+        <v>5543</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>5525</v>
+      <c r="A37" s="1">
+        <v>5552</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>5543</v>
+      <c r="A38" s="1">
+        <v>5555</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>5552</v>
+      <c r="A39" s="1">
+        <v>5564</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -722,7 +715,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>5555</v>
+        <v>5597</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -730,47 +723,47 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>5564</v>
+        <v>5598</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>5607</v>
+        <v>5604</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>5637</v>
+        <v>5605</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>5641</v>
+      <c r="A44" s="1">
+        <v>5607</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>5642</v>
+        <v>5608</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>5647</v>
+        <v>5610</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -778,15 +771,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>5656</v>
+        <v>5611</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>5662</v>
+        <v>5612</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -794,7 +787,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>5672</v>
+        <v>5613</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -802,15 +795,15 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>5674</v>
+        <v>5614</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>5676</v>
+        <v>5615</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -818,39 +811,39 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>5688</v>
+        <v>5616</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>5708</v>
+        <v>5619</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>5710</v>
+        <v>5620</v>
       </c>
       <c r="B54">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>5711</v>
+        <v>5621</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>5720</v>
+        <v>5622</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -858,95 +851,103 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>5724</v>
+        <v>5623</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>5728</v>
+        <v>5624</v>
       </c>
       <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>5625</v>
+      </c>
+      <c r="B59">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>5597</v>
+        <v>5626</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>5598</v>
+        <v>5627</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>5604</v>
+        <v>5628</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>5605</v>
+        <v>5629</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>5607</v>
+        <v>5630</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>5608</v>
+        <v>5631</v>
       </c>
       <c r="B65">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>5610</v>
+        <v>5632</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>5611</v>
+        <v>5633</v>
       </c>
       <c r="B67">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>5612</v>
+        <v>5634</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>5613</v>
+        <v>5635</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -954,15 +955,15 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>5614</v>
+        <v>5636</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>5615</v>
+      <c r="A71" s="1">
+        <v>5637</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -970,127 +971,127 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>5616</v>
+        <v>5638</v>
       </c>
       <c r="B72">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>5619</v>
+        <v>5639</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>5620</v>
+        <v>5640</v>
       </c>
       <c r="B74">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>5621</v>
+      <c r="A75" s="1">
+        <v>5641</v>
       </c>
       <c r="B75">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>5622</v>
+      <c r="A76" s="1">
+        <v>5642</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>5623</v>
+        <v>5643</v>
       </c>
       <c r="B77">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>5624</v>
+        <v>5644</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>5625</v>
+        <v>5645</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>5626</v>
+        <v>5646</v>
       </c>
       <c r="B80">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>5627</v>
+      <c r="A81" s="1">
+        <v>5647</v>
       </c>
       <c r="B81">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>5628</v>
+        <v>5648</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>5629</v>
+        <v>5649</v>
       </c>
       <c r="B83">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>5630</v>
+        <v>5650</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>5631</v>
+        <v>5651</v>
       </c>
       <c r="B85">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>5632</v>
+        <v>5652</v>
       </c>
       <c r="B86">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>5633</v>
+        <v>5653</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -1098,31 +1099,31 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>5634</v>
+        <v>5654</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>5635</v>
+        <v>5655</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>5636</v>
+      <c r="A90" s="1">
+        <v>5656</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>5637</v>
+        <v>5657</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1130,7 +1131,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>5638</v>
+        <v>5658</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -1138,111 +1139,111 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>5639</v>
+        <v>5659</v>
       </c>
       <c r="B93">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>5640</v>
+        <v>5660</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>5641</v>
+        <v>5661</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>5642</v>
+      <c r="A96" s="1">
+        <v>5662</v>
       </c>
       <c r="B96">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>5643</v>
+        <v>5663</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>5644</v>
+        <v>5664</v>
       </c>
       <c r="B98">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>5645</v>
+        <v>5665</v>
       </c>
       <c r="B99">
-        <v>69</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>5646</v>
+        <v>5666</v>
       </c>
       <c r="B100">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>5647</v>
+        <v>5667</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>5648</v>
+        <v>5668</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>5649</v>
+        <v>5669</v>
       </c>
       <c r="B103">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>5650</v>
+        <v>5670</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>5651</v>
+        <v>5671</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106">
-        <v>5652</v>
+      <c r="A106" s="1">
+        <v>5672</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -1250,31 +1251,31 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>5653</v>
+        <v>5673</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <v>5654</v>
+      <c r="A108" s="1">
+        <v>5674</v>
       </c>
       <c r="B108">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>5655</v>
+        <v>5675</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>5656</v>
+      <c r="A110" s="1">
+        <v>5676</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -1282,39 +1283,39 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>5657</v>
+        <v>5677</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>5658</v>
+        <v>5678</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>5659</v>
+        <v>5679</v>
       </c>
       <c r="B113">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>5660</v>
+        <v>5680</v>
       </c>
       <c r="B114">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>5661</v>
+        <v>5681</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -1322,359 +1323,359 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>5662</v>
+        <v>5682</v>
       </c>
       <c r="B116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>5663</v>
+        <v>5683</v>
       </c>
       <c r="B117">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>5664</v>
+        <v>5684</v>
       </c>
       <c r="B118">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>5665</v>
+        <v>5685</v>
       </c>
       <c r="B119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>5666</v>
+        <v>5686</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>5667</v>
+        <v>5687</v>
       </c>
       <c r="B121">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122">
-        <v>5668</v>
+      <c r="A122" s="1">
+        <v>5688</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>5669</v>
+        <v>5689</v>
       </c>
       <c r="B123">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>5670</v>
+        <v>5690</v>
       </c>
       <c r="B124">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>5671</v>
+        <v>5691</v>
       </c>
       <c r="B125">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>5672</v>
+        <v>5692</v>
       </c>
       <c r="B126">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>5673</v>
+        <v>5693</v>
       </c>
       <c r="B127">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>5674</v>
+        <v>5694</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>5675</v>
+        <v>5695</v>
       </c>
       <c r="B129">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>5676</v>
+        <v>5696</v>
       </c>
       <c r="B130">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>5677</v>
+        <v>5697</v>
       </c>
       <c r="B131">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>5678</v>
+        <v>5698</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>5679</v>
+        <v>5699</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>5680</v>
+        <v>5700</v>
       </c>
       <c r="B134">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135">
-        <v>5681</v>
+        <v>5701</v>
       </c>
       <c r="B135">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
-        <v>5682</v>
+        <v>5702</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>5683</v>
+        <v>5703</v>
       </c>
       <c r="B137">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>5684</v>
+        <v>5704</v>
       </c>
       <c r="B138">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>5685</v>
+        <v>5705</v>
       </c>
       <c r="B139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>5686</v>
+        <v>5706</v>
       </c>
       <c r="B140">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>5687</v>
+        <v>5707</v>
       </c>
       <c r="B141">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142">
-        <v>5688</v>
+      <c r="A142" s="1">
+        <v>5708</v>
       </c>
       <c r="B142">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>5689</v>
+        <v>5709</v>
       </c>
       <c r="B143">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144">
-        <v>5690</v>
+      <c r="A144" s="1">
+        <v>5710</v>
       </c>
       <c r="B144">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145">
-        <v>5691</v>
+      <c r="A145" s="1">
+        <v>5711</v>
       </c>
       <c r="B145">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>5692</v>
+        <v>5712</v>
       </c>
       <c r="B146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>5693</v>
+        <v>5713</v>
       </c>
       <c r="B147">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>5694</v>
+        <v>5714</v>
       </c>
       <c r="B148">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>5695</v>
+        <v>5715</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150">
-        <v>5696</v>
+        <v>5716</v>
       </c>
       <c r="B150">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>5697</v>
+        <v>5717</v>
       </c>
       <c r="B151">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>5698</v>
+        <v>5718</v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>5699</v>
+        <v>5719</v>
       </c>
       <c r="B153">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154">
-        <v>5700</v>
+      <c r="A154" s="1">
+        <v>5720</v>
       </c>
       <c r="B154">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>5701</v>
+        <v>5721</v>
       </c>
       <c r="B155">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>5702</v>
+        <v>5722</v>
       </c>
       <c r="B156">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>5703</v>
+        <v>5723</v>
       </c>
       <c r="B157">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158">
-        <v>5704</v>
+      <c r="A158" s="1">
+        <v>5724</v>
       </c>
       <c r="B158">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159">
-        <v>5705</v>
+        <v>5725</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160">
-        <v>5706</v>
+        <v>5726</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -1682,15 +1683,15 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161">
-        <v>5707</v>
+        <v>5727</v>
       </c>
       <c r="B161">
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162">
-        <v>5708</v>
+      <c r="A162" s="1">
+        <v>5728</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -1698,251 +1699,81 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163">
-        <v>5709</v>
+        <v>5729</v>
       </c>
       <c r="B163">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164">
-        <v>5710</v>
+        <v>5730</v>
       </c>
       <c r="B164">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165">
-        <v>5711</v>
+        <v>5731</v>
       </c>
       <c r="B165">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166">
-        <v>5712</v>
+        <v>5732</v>
       </c>
       <c r="B166">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167">
-        <v>5713</v>
+        <v>5733</v>
       </c>
       <c r="B167">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168">
-        <v>5714</v>
+        <v>5734</v>
       </c>
       <c r="B168">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169">
-        <v>5715</v>
+        <v>5735</v>
       </c>
       <c r="B169">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170">
-        <v>5716</v>
+        <v>5736</v>
       </c>
       <c r="B170">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171">
-        <v>5717</v>
-      </c>
-      <c r="B171">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172">
-        <v>5718</v>
-      </c>
-      <c r="B172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173">
-        <v>5719</v>
-      </c>
-      <c r="B173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174">
-        <v>5720</v>
-      </c>
-      <c r="B174">
+        <v>5738</v>
+      </c>
+      <c r="B171" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175">
-        <v>5721</v>
-      </c>
-      <c r="B175">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176">
-        <v>5722</v>
-      </c>
-      <c r="B176">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177">
-        <v>5723</v>
-      </c>
-      <c r="B177">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A178">
-        <v>5724</v>
-      </c>
-      <c r="B178">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179">
-        <v>5725</v>
-      </c>
-      <c r="B179">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A180">
-        <v>5726</v>
-      </c>
-      <c r="B180">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181">
-        <v>5727</v>
-      </c>
-      <c r="B181">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A182">
-        <v>5728</v>
-      </c>
-      <c r="B182">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A183">
-        <v>5729</v>
-      </c>
-      <c r="B183">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A184">
-        <v>5730</v>
-      </c>
-      <c r="B184">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185">
-        <v>5731</v>
-      </c>
-      <c r="B185">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A186">
-        <v>5732</v>
-      </c>
-      <c r="B186">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A187">
-        <v>5733</v>
-      </c>
-      <c r="B187">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A188">
-        <v>5734</v>
-      </c>
-      <c r="B188">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A189">
-        <v>5735</v>
-      </c>
-      <c r="B189">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A190">
-        <v>5736</v>
-      </c>
-      <c r="B190">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A191">
-        <v>5738</v>
-      </c>
-      <c r="B191" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A192">
-        <v>5739</v>
-      </c>
-      <c r="B192" t="s">
-        <v>2</v>
-      </c>
-      <c r="C192">
-        <v>118</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:C58">
-    <sortCondition ref="A2:A58"/>
+  <sortState ref="A2:B181">
+    <sortCondition ref="A2:A181"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>